<commit_message>
Add Chicago RADAR ARTnet Parametrization Script
</commit_message>
<xml_diff>
--- a/Analysis/Chicago_NetParams_Validation.xlsx
+++ b/Analysis/Chicago_NetParams_Validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\EpiModel Lab\ARTnet RADAR Mean Degree Comparison\ARTnet-RADAR\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{296E9AA7-F534-441E-8AF3-FC3AFCD4CBCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB64CADA-391C-4690-8FBF-A35A493B1D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,16 @@
     <sheet name="T1" sheetId="1" r:id="rId1"/>
     <sheet name="T1v2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -31,7 +37,7 @@
     <author>Connor Van Meter</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{3AEE97DF-87EF-450B-9C08-93BC0F6513B8}">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{3AEE97DF-87EF-450B-9C08-93BC0F6513B8}">
       <text>
         <r>
           <rPr>
@@ -55,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{9E847944-3F53-4531-89AD-BBD9E56F889B}">
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{9E847944-3F53-4531-89AD-BBD9E56F889B}">
       <text>
         <r>
           <rPr>
@@ -79,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{9EC75740-435E-4DFF-AD6D-F900AC468C08}">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{9EC75740-435E-4DFF-AD6D-F900AC468C08}">
       <text>
         <r>
           <rPr>
@@ -103,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{FAFBDE53-4785-4BC4-B518-F92DD0BA00D5}">
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{FAFBDE53-4785-4BC4-B518-F92DD0BA00D5}">
       <text>
         <r>
           <rPr>
@@ -151,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{82F751F3-7B0D-4DD4-BC78-0553263953A6}">
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{82F751F3-7B0D-4DD4-BC78-0553263953A6}">
       <text>
         <r>
           <rPr>
@@ -175,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{9CDEEFC2-5517-4949-B430-4BFA9CF51F46}">
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{9CDEEFC2-5517-4949-B430-4BFA9CF51F46}">
       <text>
         <r>
           <rPr>
@@ -199,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{DD22C88E-E335-42A9-B38E-A9942F8C7A43}">
+    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{DD22C88E-E335-42A9-B38E-A9942F8C7A43}">
       <text>
         <r>
           <rPr>
@@ -223,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J26" authorId="0" shapeId="0" xr:uid="{AACBC661-CF0E-49E2-86EA-B2D111E75D28}">
+    <comment ref="N26" authorId="0" shapeId="0" xr:uid="{AACBC661-CF0E-49E2-86EA-B2D111E75D28}">
       <text>
         <r>
           <rPr>
@@ -247,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J30" authorId="0" shapeId="0" xr:uid="{95091133-B49A-4C79-8444-DD2E2DC78C02}">
+    <comment ref="N30" authorId="0" shapeId="0" xr:uid="{95091133-B49A-4C79-8444-DD2E2DC78C02}">
       <text>
         <r>
           <rPr>
@@ -271,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J32" authorId="0" shapeId="0" xr:uid="{A4E920F7-9105-4EC9-9B1B-66A069D171A6}">
+    <comment ref="N32" authorId="0" shapeId="0" xr:uid="{A4E920F7-9105-4EC9-9B1B-66A069D171A6}">
       <text>
         <r>
           <rPr>
@@ -295,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J39" authorId="0" shapeId="0" xr:uid="{85649896-69D2-446F-B912-EA58E2DFE0E5}">
+    <comment ref="N39" authorId="0" shapeId="0" xr:uid="{85649896-69D2-446F-B912-EA58E2DFE0E5}">
       <text>
         <r>
           <rPr>
@@ -319,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J41" authorId="0" shapeId="0" xr:uid="{08A2BF65-7B01-420C-9C9D-C995F8E7D4A7}">
+    <comment ref="N41" authorId="0" shapeId="0" xr:uid="{08A2BF65-7B01-420C-9C9D-C995F8E7D4A7}">
       <text>
         <r>
           <rPr>
@@ -367,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{4C4FF74D-816E-48FA-8F9A-249E27DE3923}">
+    <comment ref="H47" authorId="0" shapeId="0" xr:uid="{4C4FF74D-816E-48FA-8F9A-249E27DE3923}">
       <text>
         <r>
           <rPr>
@@ -396,7 +402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="82">
   <si>
     <t>San Francisco</t>
   </si>
@@ -849,6 +855,14 @@
     <t>Discrepancies in 
 ARTnet Params</t>
   </si>
+  <si>
+    <t>Output - 
+from ARTnet Workflow</t>
+  </si>
+  <si>
+    <t>NetParams -
+from ARTnet Workflow</t>
+  </si>
 </sst>
 </file>
 
@@ -858,7 +872,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -971,6 +985,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1036,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1199,6 +1219,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1220,19 +1255,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1704,48 +1739,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64" t="s">
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64" t="s">
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -3042,1191 +3077,1688 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29583D5-FBDA-9342-8890-DEB7B7EC6DF8}">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.83203125" style="28" customWidth="1"/>
-    <col min="5" max="5" width="1.83203125" style="28" customWidth="1"/>
-    <col min="6" max="8" width="14.83203125" style="28" customWidth="1"/>
-    <col min="9" max="9" width="1.5" style="28" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="13.25" style="28" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11" style="28"/>
+    <col min="2" max="2" width="14.83203125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="28" customWidth="1"/>
+    <col min="5" max="6" width="14.83203125" style="28" customWidth="1"/>
+    <col min="7" max="7" width="1.83203125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="28" customWidth="1"/>
+    <col min="9" max="9" width="17" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="28" customWidth="1"/>
+    <col min="11" max="12" width="14.83203125" style="28" customWidth="1"/>
+    <col min="13" max="13" width="1.5" style="28" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="28" customWidth="1"/>
+    <col min="15" max="15" width="17" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" style="28" customWidth="1"/>
+    <col min="17" max="17" width="13.25" style="28" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="11" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="29" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:18" s="29" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-    </row>
-    <row r="2" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+    </row>
+    <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="70" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
       <c r="I2" s="31"/>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="31"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-    </row>
-    <row r="3" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="66"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+    </row>
+    <row r="3" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="71"/>
       <c r="B3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="F3" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="32" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="I3" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="L3" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="32" t="s">
+      <c r="M3" s="33"/>
+      <c r="N3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="O3" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q3" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="69" t="s">
+      <c r="R3" s="62" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+    </row>
+    <row r="5" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="37" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="51">
         <v>0.44</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67">
+      <c r="C5" s="60">
+        <v>198.01769999999999</v>
+      </c>
+      <c r="D5" s="60">
+        <f>2*C5/1000</f>
+        <v>0.39603539999999998</v>
+      </c>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60">
         <v>0.45</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="51">
+      <c r="G5" s="36"/>
+      <c r="H5" s="51">
         <v>0.34</v>
       </c>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67">
+      <c r="I5" s="60">
+        <v>175.43430000000001</v>
+      </c>
+      <c r="J5" s="60">
+        <f>2*I5/1000</f>
+        <v>0.35086860000000003</v>
+      </c>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60">
         <v>0.35</v>
       </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="52">
+      <c r="M5" s="36"/>
+      <c r="N5" s="52">
         <v>5.5E-2</v>
       </c>
-      <c r="L5" s="28">
+      <c r="O5" s="60">
+        <v>27.33192</v>
+      </c>
+      <c r="P5" s="76">
+        <f>2*O5/1000</f>
+        <v>5.4663839999999998E-2</v>
+      </c>
+      <c r="R5" s="28">
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
         <v>71</v>
       </c>
       <c r="B6" s="35"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="48"/>
-    </row>
-    <row r="7" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+    </row>
+    <row r="7" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="38" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="51">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67">
+      <c r="C7" s="75">
+        <v>13.72565</v>
+      </c>
+      <c r="D7" s="60">
+        <f>2*C7/1000</f>
+        <v>2.7451300000000001E-2</v>
+      </c>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60">
         <v>0.26</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="51">
+      <c r="G7" s="36"/>
+      <c r="H7" s="51">
         <v>0.26</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67">
+      <c r="I7" s="75">
+        <v>13.463229999999999</v>
+      </c>
+      <c r="J7" s="60">
+        <f>I7*2/1000</f>
+        <v>2.6926459999999999E-2</v>
+      </c>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60">
         <v>0.23</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="52">
+      <c r="M7" s="36"/>
+      <c r="N7" s="52">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="L7" s="28">
+      <c r="O7" s="75">
+        <v>1.70374</v>
+      </c>
+      <c r="P7" s="76">
+        <f>2*O7/1000</f>
+        <v>3.4074800000000001E-3</v>
+      </c>
+      <c r="R7" s="28">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="51">
         <v>0.45</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67">
+      <c r="C8" s="75">
+        <v>58.129510000000003</v>
+      </c>
+      <c r="D8" s="60">
+        <f>2*C8/1000</f>
+        <v>0.11625902</v>
+      </c>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60">
         <v>0.45</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="51">
+      <c r="G8" s="36"/>
+      <c r="H8" s="51">
         <v>0.33</v>
       </c>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67">
+      <c r="I8" s="75">
+        <v>43.55001</v>
+      </c>
+      <c r="J8" s="60">
+        <f>I8*2/1000</f>
+        <v>8.710002E-2</v>
+      </c>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60">
         <v>0.34</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="52">
+      <c r="M8" s="36"/>
+      <c r="N8" s="52">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="L8" s="28">
+      <c r="O8" s="75">
+        <v>7.7867899999999999</v>
+      </c>
+      <c r="P8" s="76">
+        <f>2*O8/1000</f>
+        <v>1.557358E-2</v>
+      </c>
+      <c r="R8" s="28">
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="38" t="s">
         <v>67</v>
       </c>
       <c r="B9" s="51">
         <v>0.51</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67">
+      <c r="C9" s="75">
+        <v>47.516379999999998</v>
+      </c>
+      <c r="D9" s="60">
+        <f>2*C9/1000</f>
+        <v>9.5032759999999994E-2</v>
+      </c>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60">
         <v>0.52</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="51">
+      <c r="G9" s="36"/>
+      <c r="H9" s="51">
         <v>0.38</v>
       </c>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67">
+      <c r="I9" s="75">
+        <v>36.967269999999999</v>
+      </c>
+      <c r="J9" s="60">
+        <f>I9*2/1000</f>
+        <v>7.3934539999999993E-2</v>
+      </c>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60">
         <v>0.42</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="52">
+      <c r="M9" s="36"/>
+      <c r="N9" s="52">
         <v>0.06</v>
       </c>
-      <c r="L9" s="28">
+      <c r="O9" s="75">
+        <v>5.9256880000000001</v>
+      </c>
+      <c r="P9" s="76">
+        <f>2*O9/1000</f>
+        <v>1.1851376E-2</v>
+      </c>
+      <c r="R9" s="28">
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="35"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="48"/>
-    </row>
-    <row r="11" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+    </row>
+    <row r="11" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="38" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="51">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67">
+      <c r="C11" s="75">
+        <v>80.552679999999995</v>
+      </c>
+      <c r="D11" s="60">
+        <f>2*C11/1000</f>
+        <v>0.16110536</v>
+      </c>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60">
         <v>0.27</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="51">
+      <c r="G11" s="36"/>
+      <c r="H11" s="51">
         <v>0.37</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67">
+      <c r="I11" s="75">
+        <v>108.0925</v>
+      </c>
+      <c r="J11" s="60">
+        <f>I11*2/1000</f>
+        <v>0.21618500000000002</v>
+      </c>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60">
         <v>0.47</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="52">
+      <c r="M11" s="36"/>
+      <c r="N11" s="52">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="L11" s="28">
+      <c r="O11" s="75">
+        <v>16.223279999999999</v>
+      </c>
+      <c r="P11" s="76">
+        <f>2*O11/1000</f>
+        <v>3.2446559999999999E-2</v>
+      </c>
+      <c r="R11" s="28">
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="38" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="51">
         <v>0.41</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67">
+      <c r="C12" s="75">
+        <v>120.24052</v>
+      </c>
+      <c r="D12" s="60">
+        <f>2*C12/1000</f>
+        <v>0.24048104000000001</v>
+      </c>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60">
         <v>0.42</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="51">
+      <c r="G12" s="36"/>
+      <c r="H12" s="51">
         <v>0.36</v>
       </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67">
+      <c r="I12" s="75">
+        <v>105.5459</v>
+      </c>
+      <c r="J12" s="60">
+        <f>I12*2/1000</f>
+        <v>0.2110918</v>
+      </c>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60">
         <v>0.38</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="52">
+      <c r="M12" s="36"/>
+      <c r="N12" s="52">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="L12" s="28">
+      <c r="O12" s="75">
+        <v>14.70431</v>
+      </c>
+      <c r="P12" s="76">
+        <f>2*O12/1000</f>
+        <v>2.940862E-2</v>
+      </c>
+      <c r="R12" s="28">
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="51">
         <v>0.47</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67">
+      <c r="C13" s="75">
+        <v>195.24216999999999</v>
+      </c>
+      <c r="D13" s="60">
+        <f>2*C13/1000</f>
+        <v>0.39048433999999999</v>
+      </c>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60">
         <v>0.46</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="51">
+      <c r="G13" s="36"/>
+      <c r="H13" s="51">
         <v>0.33</v>
       </c>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67">
+      <c r="I13" s="75">
+        <v>137.2302</v>
+      </c>
+      <c r="J13" s="60">
+        <f>I13*2/1000</f>
+        <v>0.27446039999999999</v>
+      </c>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60">
         <v>0.34</v>
       </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="52">
+      <c r="M13" s="36"/>
+      <c r="N13" s="52">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="L13" s="28">
+      <c r="O13" s="75">
+        <v>23.736249999999998</v>
+      </c>
+      <c r="P13" s="76">
+        <f>2*O13/1000</f>
+        <v>4.7472499999999994E-2</v>
+      </c>
+      <c r="R13" s="28">
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
         <v>75</v>
       </c>
       <c r="B14" s="35"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="48"/>
-    </row>
-    <row r="15" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+    </row>
+    <row r="15" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
         <v>76</v>
       </c>
       <c r="B15" s="51">
         <v>0.44</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67">
+      <c r="C15" s="75">
+        <v>358.50112000000001</v>
+      </c>
+      <c r="D15" s="60">
+        <f>2*C15/1000</f>
+        <v>0.71700224000000001</v>
+      </c>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60">
         <v>0.44</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="51">
+      <c r="G15" s="36"/>
+      <c r="H15" s="51">
         <v>0.34</v>
       </c>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67">
+      <c r="I15" s="75">
+        <v>0.67910689999999996</v>
+      </c>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60">
         <v>0.35</v>
       </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="52">
+      <c r="M15" s="36"/>
+      <c r="N15" s="52">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="L15" s="28">
+      <c r="O15" s="75">
+        <v>0.11712740000000001</v>
+      </c>
+      <c r="P15" s="61"/>
+      <c r="R15" s="28">
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="51">
         <v>0.57999999999999996</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67">
+      <c r="C16" s="75">
+        <v>41.140270000000001</v>
+      </c>
+      <c r="D16" s="60">
+        <f>2*C16/1000</f>
+        <v>8.2280539999999999E-2</v>
+      </c>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60">
         <v>0.52</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="51">
+      <c r="G16" s="36"/>
+      <c r="H16" s="51">
         <v>0.44</v>
       </c>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67">
+      <c r="I16" s="75">
+        <v>1.0879239999999999</v>
+      </c>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60">
         <v>0.48</v>
       </c>
-      <c r="I16" s="36"/>
-      <c r="J16" s="52">
+      <c r="M16" s="36"/>
+      <c r="N16" s="52">
         <v>0.14199999999999999</v>
       </c>
-      <c r="L16" s="28">
+      <c r="O16" s="75">
+        <v>0.24407209999999999</v>
+      </c>
+      <c r="P16" s="61"/>
+      <c r="R16" s="28">
         <v>0.14199999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="37" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="48"/>
-    </row>
-    <row r="18" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="61"/>
+      <c r="P17" s="61"/>
+    </row>
+    <row r="18" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="38">
         <v>0</v>
       </c>
       <c r="B18" s="53">
         <v>0.51</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36">
+      <c r="C18" s="75">
+        <v>0.45726240000000001</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36">
         <v>0.51</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="53">
+      <c r="G18" s="36"/>
+      <c r="H18" s="53">
         <v>0.46</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30">
+      <c r="I18" s="75">
+        <v>0.82923340000000001</v>
+      </c>
+      <c r="J18" s="40"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30">
         <v>0.46</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="48" t="s">
+      <c r="M18" s="36"/>
+      <c r="N18" s="48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+    </row>
+    <row r="19" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="38">
         <v>1</v>
       </c>
       <c r="B19" s="53">
         <v>0.3</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36">
+      <c r="C19" s="75">
+        <v>0.36523099999999997</v>
+      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36">
         <v>0.32</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="53">
+      <c r="G19" s="36"/>
+      <c r="H19" s="53">
         <v>0.18</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30">
+      <c r="I19" s="75">
+        <v>0.5267579</v>
+      </c>
+      <c r="J19" s="40"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30">
         <v>0.21</v>
       </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="48" t="s">
+      <c r="M19" s="36"/>
+      <c r="N19" s="48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O19" s="61"/>
+      <c r="P19" s="61"/>
+    </row>
+    <row r="20" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="38">
         <v>2</v>
       </c>
       <c r="B20" s="53">
         <v>0.18</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36">
+      <c r="C20" s="75">
+        <v>0.29172239999999999</v>
+      </c>
+      <c r="D20" s="40"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36">
         <v>0.2</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="53">
+      <c r="G20" s="36"/>
+      <c r="H20" s="53">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30">
+      <c r="I20" s="75">
+        <v>0.334615</v>
+      </c>
+      <c r="J20" s="40"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30">
         <v>0.09</v>
       </c>
-      <c r="I20" s="40"/>
-      <c r="J20" s="48" t="s">
+      <c r="M20" s="40"/>
+      <c r="N20" s="48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O20" s="61"/>
+      <c r="P20" s="61"/>
+    </row>
+    <row r="21" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="38">
         <v>3</v>
       </c>
       <c r="B21" s="53">
         <v>0.1</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36">
+      <c r="C21" s="75">
+        <v>0.23300860000000001</v>
+      </c>
+      <c r="D21" s="40"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36">
         <v>0.12</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="53" t="s">
+      <c r="G21" s="36"/>
+      <c r="H21" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="48" t="s">
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O21" s="61"/>
+      <c r="P21" s="61"/>
+    </row>
+    <row r="22" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="34" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="52">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68">
+      <c r="C22" s="75">
+        <v>1.6393439999999999E-2</v>
+      </c>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61">
         <v>3.1E-2</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="52">
+      <c r="G22" s="40"/>
+      <c r="H22" s="52">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68">
+      <c r="I22" s="75">
+        <v>0.2021858</v>
+      </c>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48" t="s">
+      <c r="M22" s="48"/>
+      <c r="N22" s="48" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O22" s="61"/>
+      <c r="P22" s="61"/>
+    </row>
+    <row r="23" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="34" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="36"/>
       <c r="F23" s="36"/>
       <c r="G23" s="36"/>
       <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-    </row>
-    <row r="24" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+    </row>
+    <row r="24" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="37" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="53">
         <v>0.47</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36">
-        <v>0.47</v>
-      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="36"/>
       <c r="F24" s="36">
+        <v>0.47</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36">
         <v>0.34</v>
       </c>
-      <c r="G24" s="55">
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="55">
         <v>0.38</v>
       </c>
-      <c r="H24" s="28">
+      <c r="L24" s="28">
         <v>0.38</v>
       </c>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36">
+      <c r="M24" s="36"/>
+      <c r="N24" s="36">
         <v>0.4</v>
       </c>
-      <c r="K24" s="58">
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="58">
         <v>0.39</v>
       </c>
-      <c r="L24" s="28">
+      <c r="R24" s="28">
         <v>0.39</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="37" t="s">
         <v>70</v>
       </c>
       <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="36"/>
       <c r="F25" s="36"/>
       <c r="G25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-    </row>
-    <row r="26" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H25" s="36"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+    </row>
+    <row r="26" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="38" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="53">
         <v>0.61</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36">
-        <v>0.61</v>
-      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
       <c r="E26" s="36"/>
       <c r="F26" s="36">
+        <v>0.61</v>
+      </c>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36">
         <v>0.43</v>
       </c>
-      <c r="G26" s="55">
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="55">
         <v>0.46</v>
       </c>
-      <c r="H26" s="28">
+      <c r="L26" s="28">
         <v>0.46</v>
       </c>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36">
+      <c r="M26" s="36"/>
+      <c r="N26" s="36">
         <v>0.43</v>
       </c>
-      <c r="K26" s="58">
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="58">
         <v>0.42</v>
       </c>
-      <c r="L26" s="28">
+      <c r="R26" s="28">
         <v>0.42</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B27" s="36">
         <v>0.51</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="55">
         <v>0.5</v>
       </c>
-      <c r="D27" s="28">
+      <c r="F27" s="28">
         <v>0.5</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36">
+      <c r="G27" s="36"/>
+      <c r="H27" s="36">
         <v>0.36</v>
       </c>
-      <c r="G27" s="55">
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="55">
         <v>0.4</v>
       </c>
-      <c r="H27" s="28">
+      <c r="L27" s="28">
         <v>0.4</v>
       </c>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36">
+      <c r="M27" s="36"/>
+      <c r="N27" s="36">
         <v>0.4</v>
       </c>
-      <c r="K27" s="58">
+      <c r="O27" s="40"/>
+      <c r="P27" s="40"/>
+      <c r="Q27" s="58">
         <v>0.39</v>
       </c>
-      <c r="L27" s="28">
+      <c r="R27" s="28">
         <v>0.39</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="38" t="s">
         <v>67</v>
       </c>
       <c r="B28" s="53">
         <v>0.4</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="28">
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="28">
         <v>0.4</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36">
+      <c r="G28" s="36"/>
+      <c r="H28" s="36">
         <v>0.31</v>
       </c>
-      <c r="G28" s="55">
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="55">
         <v>0.34</v>
       </c>
-      <c r="H28" s="28">
+      <c r="L28" s="28">
         <v>0.34</v>
       </c>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36">
+      <c r="M28" s="36"/>
+      <c r="N28" s="36">
         <v>0.38</v>
       </c>
-      <c r="K28" s="58">
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="58">
         <v>0.37</v>
       </c>
-      <c r="L28" s="28">
+      <c r="R28" s="28">
         <v>0.37</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="34" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
       <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
       <c r="G29" s="36"/>
       <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-    </row>
-    <row r="30" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+    </row>
+    <row r="30" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="37" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="53">
         <v>0.51</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="28">
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="28">
         <v>0.51</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="53">
+      <c r="G30" s="36"/>
+      <c r="H30" s="53">
         <v>0.56999999999999995</v>
       </c>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36">
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I30" s="36"/>
-      <c r="J30" s="53">
+      <c r="M30" s="36"/>
+      <c r="N30" s="53">
         <v>0.66</v>
       </c>
-      <c r="L30" s="28">
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="R30" s="28">
         <v>0.65</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="37" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
       <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
       <c r="G31" s="36"/>
       <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-    </row>
-    <row r="32" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+    </row>
+    <row r="32" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="38" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="53">
         <v>0.23</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="28">
+      <c r="C32" s="75">
+        <v>0.40107670000000001</v>
+      </c>
+      <c r="D32" s="40"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="28">
         <v>0.27</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36">
+      <c r="G32" s="36"/>
+      <c r="H32" s="36">
         <v>0.42</v>
       </c>
-      <c r="G32" s="55">
+      <c r="I32" s="75">
+        <v>0.44767420000000002</v>
+      </c>
+      <c r="J32" s="40"/>
+      <c r="K32" s="55">
         <v>0.41</v>
       </c>
-      <c r="H32" s="28">
+      <c r="L32" s="28">
         <v>0.47</v>
       </c>
-      <c r="I32" s="36"/>
-      <c r="J32" s="53">
+      <c r="M32" s="36"/>
+      <c r="N32" s="53">
         <v>0.41</v>
       </c>
-      <c r="L32" s="28">
+      <c r="O32" s="75">
+        <v>0.40556799999999998</v>
+      </c>
+      <c r="P32" s="40"/>
+      <c r="R32" s="28">
         <v>0.41</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="38" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="53">
         <v>0.28999999999999998</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="28">
+      <c r="C33" s="75">
+        <v>0.30947669999999999</v>
+      </c>
+      <c r="D33" s="40"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="28">
         <v>0.42</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="53">
+      <c r="G33" s="36"/>
+      <c r="H33" s="53">
         <v>0.32</v>
       </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="28">
+      <c r="I33" s="75">
+        <v>0.34958980000000001</v>
+      </c>
+      <c r="J33" s="40"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="28">
         <v>0.38</v>
       </c>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36">
+      <c r="M33" s="36"/>
+      <c r="N33" s="36">
         <v>0.35</v>
       </c>
-      <c r="K33" s="58">
+      <c r="O33" s="75">
+        <v>0.35109400000000002</v>
+      </c>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="58">
         <v>0.34</v>
       </c>
-      <c r="L33" s="28">
+      <c r="R33" s="28">
         <v>0.32</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="38" t="s">
         <v>47</v>
       </c>
       <c r="B34" s="36">
         <v>0.64</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="75">
+        <v>0.70304710000000004</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="55">
         <v>0.65</v>
       </c>
-      <c r="D34" s="28">
+      <c r="F34" s="28">
         <v>0.46</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36">
+      <c r="G34" s="36"/>
+      <c r="H34" s="36">
         <v>0.67</v>
       </c>
-      <c r="G34" s="55">
+      <c r="I34" s="75">
+        <v>0.68170520000000001</v>
+      </c>
+      <c r="J34" s="40"/>
+      <c r="K34" s="55">
         <v>0.68</v>
       </c>
-      <c r="H34" s="28">
+      <c r="L34" s="28">
         <v>0.34</v>
       </c>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36">
+      <c r="M34" s="36"/>
+      <c r="N34" s="36">
         <v>0.71</v>
       </c>
-      <c r="K34" s="58">
+      <c r="O34" s="75">
+        <v>0.70599509999999999</v>
+      </c>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="58">
         <v>0.7</v>
       </c>
-      <c r="L34" s="28">
+      <c r="R34" s="28">
         <v>0.7</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
       <c r="E35" s="36"/>
       <c r="F35" s="36"/>
       <c r="G35" s="36"/>
       <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-    </row>
-    <row r="36" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="36"/>
+      <c r="N35" s="36"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="40"/>
+    </row>
+    <row r="36" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="41">
         <v>0</v>
       </c>
       <c r="B36" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
       <c r="E36" s="36"/>
-      <c r="F36" s="36" t="s">
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="52">
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="52">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="L36" s="28">
+      <c r="O36" s="75">
+        <v>6.4904890000000007E-2</v>
+      </c>
+      <c r="P36" s="61"/>
+      <c r="R36" s="28">
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="41">
         <v>1</v>
       </c>
       <c r="B37" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
       <c r="E37" s="36"/>
-      <c r="F37" s="36" t="s">
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="52">
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="36"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="36"/>
+      <c r="N37" s="52">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="L37" s="28">
+      <c r="O37" s="75">
+        <v>7.6161199999999998E-2</v>
+      </c>
+      <c r="P37" s="61"/>
+      <c r="R37" s="28">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="41">
         <v>2</v>
       </c>
       <c r="B38" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
       <c r="E38" s="36"/>
-      <c r="F38" s="36" t="s">
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="52">
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="36"/>
+      <c r="N38" s="52">
         <v>0.10199999999999999</v>
       </c>
-      <c r="L38" s="28">
+      <c r="O38" s="75">
+        <v>0.16244942000000001</v>
+      </c>
+      <c r="P38" s="61"/>
+      <c r="R38" s="28">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="41" t="s">
         <v>69</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
       <c r="E39" s="36"/>
-      <c r="F39" s="36" t="s">
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="52">
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="36"/>
+      <c r="N39" s="52">
         <v>0.28499999999999998</v>
       </c>
-      <c r="L39" s="28">
+      <c r="O39" s="75">
+        <v>0.38229735999999997</v>
+      </c>
+      <c r="P39" s="61"/>
+      <c r="R39" s="28">
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="34" t="s">
         <v>60</v>
       </c>
       <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
-    </row>
-    <row r="41" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="40"/>
+    </row>
+    <row r="41" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B41" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
       <c r="E41" s="36"/>
-      <c r="F41" s="36" t="s">
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="52">
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="36"/>
+      <c r="N41" s="52">
         <v>0</v>
       </c>
-      <c r="L41" s="28">
+      <c r="O41" s="75">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P41" s="61"/>
+      <c r="R41" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="41" t="s">
         <v>54</v>
       </c>
       <c r="B42" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
       <c r="E42" s="36"/>
-      <c r="F42" s="36" t="s">
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="52">
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="36"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="52">
         <v>0</v>
       </c>
-      <c r="L42" s="28">
+      <c r="O42" s="75">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P42" s="61"/>
+      <c r="R42" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="41" t="s">
         <v>55</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
       <c r="E43" s="36"/>
-      <c r="F43" s="36" t="s">
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="52">
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
+      <c r="N43" s="52">
         <v>1.4E-2</v>
       </c>
-      <c r="L43" s="28">
+      <c r="O43" s="75">
+        <v>1.9502350000000002E-2</v>
+      </c>
+      <c r="P43" s="61"/>
+      <c r="R43" s="28">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="41" t="s">
         <v>57</v>
       </c>
       <c r="B44" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
       <c r="E44" s="36"/>
-      <c r="F44" s="36" t="s">
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="52">
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="52">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="L44" s="28">
+      <c r="O44" s="75">
+        <v>7.1233400000000002E-2</v>
+      </c>
+      <c r="P44" s="61"/>
+      <c r="R44" s="28">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="41" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
       <c r="E45" s="36"/>
-      <c r="F45" s="36" t="s">
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="52">
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="52">
         <v>0.22500000000000001</v>
       </c>
-      <c r="L45" s="28">
+      <c r="O45" s="75">
+        <v>0.54303416999999998</v>
+      </c>
+      <c r="P45" s="61"/>
+      <c r="R45" s="28">
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="46" t="s">
         <v>61</v>
       </c>
       <c r="B46" s="40"/>
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
       <c r="G46" s="36"/>
       <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
-    </row>
-    <row r="47" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="40"/>
+      <c r="P46" s="40"/>
+    </row>
+    <row r="47" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="49">
         <v>122</v>
       </c>
-      <c r="C47" s="56">
+      <c r="C47" s="73"/>
+      <c r="D47" s="73"/>
+      <c r="E47" s="56">
         <v>121.6</v>
       </c>
-      <c r="D47" s="28">
+      <c r="F47" s="28">
         <v>143.69999999999999</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="49">
+      <c r="G47" s="36"/>
+      <c r="H47" s="49">
         <v>52.4</v>
       </c>
-      <c r="G47" s="56">
+      <c r="I47" s="73"/>
+      <c r="J47" s="73"/>
+      <c r="K47" s="56">
         <v>53.2</v>
       </c>
-      <c r="H47" s="28">
+      <c r="L47" s="28">
         <v>67.3</v>
       </c>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36" t="s">
+      <c r="M47" s="36"/>
+      <c r="N47" s="36" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O47" s="40"/>
+      <c r="P47" s="40"/>
+    </row>
+    <row r="48" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="41" t="s">
         <v>62</v>
       </c>
       <c r="B48" s="49">
         <v>35.799999999999997</v>
       </c>
-      <c r="C48" s="56">
+      <c r="C48" s="73"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="56">
         <v>35.200000000000003</v>
       </c>
-      <c r="D48" s="28">
+      <c r="F48" s="28">
         <v>54.5</v>
       </c>
-      <c r="E48" s="36"/>
-      <c r="F48" s="54">
+      <c r="G48" s="36"/>
+      <c r="H48" s="54">
         <v>23.1</v>
       </c>
-      <c r="G48" s="49"/>
-      <c r="H48" s="28">
+      <c r="I48" s="73"/>
+      <c r="J48" s="73"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="28">
         <v>44.6</v>
       </c>
-      <c r="I48" s="36"/>
-      <c r="J48" s="36" t="s">
+      <c r="M48" s="36"/>
+      <c r="N48" s="36" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O48" s="40"/>
+      <c r="P48" s="40"/>
+    </row>
+    <row r="49" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="41" t="s">
         <v>63</v>
       </c>
       <c r="B49" s="49">
         <v>88.4</v>
       </c>
-      <c r="C49" s="56">
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="56">
         <v>86.9</v>
       </c>
-      <c r="D49" s="28">
+      <c r="F49" s="28">
         <v>88.4</v>
       </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="49">
+      <c r="G49" s="36"/>
+      <c r="H49" s="49">
         <v>49.7</v>
       </c>
-      <c r="G49" s="56">
+      <c r="I49" s="73"/>
+      <c r="J49" s="73"/>
+      <c r="K49" s="56">
         <v>51.2</v>
       </c>
-      <c r="H49" s="28">
+      <c r="L49" s="28">
         <v>76.3</v>
       </c>
-      <c r="I49" s="36"/>
-      <c r="J49" s="36" t="s">
+      <c r="M49" s="36"/>
+      <c r="N49" s="36" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O49" s="40"/>
+      <c r="P49" s="40"/>
+    </row>
+    <row r="50" spans="1:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="47" t="s">
         <v>64</v>
       </c>
       <c r="B50" s="50">
         <v>256.60000000000002</v>
       </c>
-      <c r="C50" s="57">
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="57">
         <v>252.3</v>
       </c>
-      <c r="D50" s="59">
+      <c r="F50" s="59">
         <v>188.7</v>
       </c>
-      <c r="E50" s="43"/>
-      <c r="F50" s="50">
+      <c r="G50" s="43"/>
+      <c r="H50" s="50">
         <v>59.1</v>
       </c>
-      <c r="G50" s="57">
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="57">
         <v>57.9</v>
       </c>
-      <c r="H50" s="59">
+      <c r="L50" s="59">
         <v>81.599999999999994</v>
       </c>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43" t="s">
+      <c r="M50" s="43"/>
+      <c r="N50" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="K50" s="59"/>
-      <c r="L50" s="59"/>
-    </row>
-    <row r="51" spans="1:12" ht="13" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="O50" s="43"/>
+      <c r="P50" s="43"/>
+      <c r="Q50" s="59"/>
+      <c r="R50" s="59"/>
+    </row>
+    <row r="51" spans="1:18" ht="13" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A51" s="42"/>
       <c r="B51" s="42"/>
       <c r="C51" s="42"/>
@@ -4237,89 +4769,131 @@
       <c r="H51" s="42"/>
       <c r="I51" s="42"/>
       <c r="J51" s="42"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K51" s="42"/>
+      <c r="L51" s="42"/>
+      <c r="M51" s="42"/>
+      <c r="N51" s="42"/>
+      <c r="O51" s="42"/>
+      <c r="P51" s="42"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="44"/>
       <c r="B52" s="44"/>
       <c r="C52" s="44"/>
       <c r="D52" s="44"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
       <c r="G52" s="42"/>
       <c r="H52" s="42"/>
       <c r="I52" s="42"/>
       <c r="J52" s="42"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
+      <c r="M52" s="42"/>
+      <c r="N52" s="42"/>
+      <c r="O52" s="42"/>
+      <c r="P52" s="42"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="44"/>
       <c r="B53" s="44"/>
       <c r="C53" s="44"/>
       <c r="D53" s="44"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
       <c r="G53" s="42"/>
       <c r="H53" s="42"/>
       <c r="I53" s="42"/>
       <c r="J53" s="42"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K53" s="42"/>
+      <c r="L53" s="42"/>
+      <c r="M53" s="42"/>
+      <c r="N53" s="42"/>
+      <c r="O53" s="42"/>
+      <c r="P53" s="42"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="44"/>
       <c r="B54" s="44"/>
       <c r="C54" s="44"/>
       <c r="D54" s="44"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
       <c r="G54" s="42"/>
       <c r="H54" s="42"/>
       <c r="I54" s="42"/>
       <c r="J54" s="42"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K54" s="42"/>
+      <c r="L54" s="42"/>
+      <c r="M54" s="42"/>
+      <c r="N54" s="42"/>
+      <c r="O54" s="42"/>
+      <c r="P54" s="42"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="44"/>
       <c r="B55" s="44"/>
       <c r="C55" s="44"/>
       <c r="D55" s="44"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
       <c r="G55" s="42"/>
       <c r="H55" s="42"/>
       <c r="I55" s="42"/>
       <c r="J55" s="42"/>
-    </row>
-    <row r="56" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="K55" s="42"/>
+      <c r="L55" s="42"/>
+      <c r="M55" s="42"/>
+      <c r="N55" s="42"/>
+      <c r="O55" s="42"/>
+      <c r="P55" s="42"/>
+    </row>
+    <row r="56" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="45"/>
       <c r="B56" s="45"/>
       <c r="C56" s="45"/>
       <c r="D56" s="45"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="42"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
       <c r="G56" s="42"/>
       <c r="H56" s="42"/>
       <c r="I56" s="42"/>
       <c r="J56" s="42"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K56" s="42"/>
+      <c r="L56" s="42"/>
+      <c r="M56" s="42"/>
+      <c r="N56" s="42"/>
+      <c r="O56" s="42"/>
+      <c r="P56" s="42"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="44"/>
       <c r="B57" s="44"/>
       <c r="C57" s="44"/>
       <c r="D57" s="44"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
       <c r="G57" s="42"/>
       <c r="H57" s="42"/>
       <c r="I57" s="42"/>
       <c r="J57" s="42"/>
-    </row>
-    <row r="59" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K57" s="42"/>
+      <c r="L57" s="42"/>
+      <c r="M57" s="42"/>
+      <c r="N57" s="42"/>
+      <c r="O57" s="42"/>
+      <c r="P57" s="42"/>
+    </row>
+    <row r="59" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="27"/>
     </row>
-    <row r="61" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>